<commit_message>
[DMA] Front-end [Joystick & memcard] Temp stuff committed. [SPU] Doc update.
</commit_message>
<xml_diff>
--- a/hdlSPU/doc/StateMachineTiming.xlsx
+++ b/hdlSPU/doc/StateMachineTiming.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="33">
   <si>
     <t>READ ADPCM</t>
   </si>
@@ -104,6 +104,18 @@
   <si>
     <t>Would be nice to rebalance the interpolator and have 6 everywhere…</t>
   </si>
+  <si>
+    <t>Need 14 Cycles only if we want to expand everything to 5 CYCLES</t>
+  </si>
+  <si>
+    <t>We can give one more cycle per channel in exchange</t>
+  </si>
+  <si>
+    <t>remains 4 cycles even with extension in reverb</t>
+  </si>
+  <si>
+    <t>Reduce from 128 to 104 cycles.</t>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -455,6 +473,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,10 +837,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S158"/>
+  <dimension ref="A1:AE158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+      <selection activeCell="H17" sqref="H17:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -824,10 +850,11 @@
     <col min="6" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="13" max="17" width="14" customWidth="1"/>
+    <col min="23" max="27" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:19">
+    <row r="1" spans="1:31" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:31" ht="15.75" thickBot="1">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -864,8 +891,23 @@
       <c r="Q2" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" thickBot="1">
       <c r="B3">
         <v>0</v>
       </c>
@@ -883,8 +925,14 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="W3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+    </row>
+    <row r="4" spans="1:31">
       <c r="B4">
         <v>1</v>
       </c>
@@ -910,8 +958,15 @@
       <c r="S4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="W4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="8"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="B5">
         <v>2</v>
       </c>
@@ -931,8 +986,15 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="W5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="8"/>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" thickBot="1">
       <c r="B6">
         <v>3</v>
       </c>
@@ -952,8 +1014,15 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="8"/>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" thickBot="1">
       <c r="B7">
         <v>4</v>
       </c>
@@ -973,8 +1042,12 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="W7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="8"/>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" thickBot="1">
       <c r="B8">
         <v>5</v>
       </c>
@@ -995,8 +1068,10 @@
         <v>2</v>
       </c>
       <c r="Q8" s="8"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W8" s="6"/>
+      <c r="AA8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" thickBot="1">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1010,8 +1085,15 @@
       <c r="I9" s="1"/>
       <c r="M9" s="6"/>
       <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="W9" s="6"/>
+      <c r="X9" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="8"/>
+    </row>
+    <row r="10" spans="1:31">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1034,8 +1116,15 @@
       <c r="S10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="W10" s="6"/>
+      <c r="X10" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="8"/>
+    </row>
+    <row r="11" spans="1:31">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1055,8 +1144,15 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="W11" s="6"/>
+      <c r="X11" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="8"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" thickBot="1">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1076,8 +1172,15 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W12" s="6"/>
+      <c r="X12" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" thickBot="1">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1097,8 +1200,15 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="W13" s="6"/>
+      <c r="X13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" thickBot="1">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1117,8 +1227,15 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W14" s="6"/>
+      <c r="X14" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" thickBot="1">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1137,8 +1254,17 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="8"/>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="W15" s="6"/>
+      <c r="X15" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+    </row>
+    <row r="16" spans="1:31">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1162,8 +1288,17 @@
       <c r="S16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="W16" s="6"/>
+      <c r="X16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+    </row>
+    <row r="17" spans="1:31">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1190,8 +1325,17 @@
         <v>1</v>
       </c>
       <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="W17" s="6"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE17" s="7"/>
+    </row>
+    <row r="18" spans="1:31" ht="15.75" thickBot="1">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1215,8 +1359,17 @@
         <v>1</v>
       </c>
       <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W18" s="6"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE18" s="7"/>
+    </row>
+    <row r="19" spans="1:31" ht="15.75" thickBot="1">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1240,8 +1393,17 @@
         <v>1</v>
       </c>
       <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="W19" s="6"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE19" s="7"/>
+    </row>
+    <row r="20" spans="1:31">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1264,8 +1426,14 @@
       <c r="Q20" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="W20" s="6"/>
+      <c r="X20" s="7"/>
+      <c r="AA20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE20" s="7"/>
+    </row>
+    <row r="21" spans="1:31" ht="15.75" thickBot="1">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1288,8 +1456,14 @@
         <v>9</v>
       </c>
       <c r="P21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W21" s="6"/>
+      <c r="X21" s="7"/>
+      <c r="AA21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE21" s="7"/>
+    </row>
+    <row r="22" spans="1:31" ht="15.75" thickBot="1">
       <c r="B22">
         <v>19</v>
       </c>
@@ -1308,8 +1482,15 @@
       </c>
       <c r="P22" s="7"/>
       <c r="Q22" s="8"/>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="W22" s="6"/>
+      <c r="X22" s="7"/>
+      <c r="Z22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA22" s="8"/>
+      <c r="AD22" s="7"/>
+    </row>
+    <row r="23" spans="1:31">
       <c r="B23">
         <v>20</v>
       </c>
@@ -1332,8 +1513,15 @@
       <c r="S23">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="W23" s="6"/>
+      <c r="X23" s="7"/>
+      <c r="Z23" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="8"/>
+      <c r="AD23" s="7"/>
+    </row>
+    <row r="24" spans="1:31">
       <c r="B24">
         <v>21</v>
       </c>
@@ -1353,8 +1541,15 @@
       </c>
       <c r="Q24" s="8"/>
       <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="W24" s="6"/>
+      <c r="X24" s="7"/>
+      <c r="Z24" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="8"/>
+      <c r="AD24" s="7"/>
+    </row>
+    <row r="25" spans="1:31" ht="15.75" thickBot="1">
       <c r="B25">
         <v>22</v>
       </c>
@@ -1371,8 +1566,15 @@
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" ht="15.75" thickBot="1">
+      <c r="W25" s="20"/>
+      <c r="X25" s="7"/>
+      <c r="Z25" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="8"/>
+      <c r="AD25" s="7"/>
+    </row>
+    <row r="26" spans="1:31" ht="15.75" thickBot="1">
       <c r="B26">
         <v>23</v>
       </c>
@@ -1389,13 +1591,14 @@
       </c>
       <c r="Q26" s="22"/>
       <c r="R26" s="1"/>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="AA26" s="22"/>
+    </row>
+    <row r="28" spans="1:31">
       <c r="N28" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15.75" thickBot="1">
+    <row r="29" spans="1:31" ht="15.75" thickBot="1">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1606,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:31">
       <c r="B30">
         <v>0</v>
       </c>
@@ -1421,8 +1624,19 @@
       <c r="M30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="W30" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="33">
+        <v>4</v>
+      </c>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="B31">
         <v>1</v>
       </c>
@@ -1436,8 +1650,15 @@
       <c r="M31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="W31" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="36"/>
+    </row>
+    <row r="32" spans="1:31">
       <c r="B32">
         <v>2</v>
       </c>
@@ -1451,8 +1672,15 @@
       <c r="N32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="2:13">
+      <c r="W32" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="36"/>
+    </row>
+    <row r="33" spans="2:27">
       <c r="B33">
         <v>3</v>
       </c>
@@ -1466,8 +1694,15 @@
       <c r="M33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="2:13">
+      <c r="W33" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="36"/>
+    </row>
+    <row r="34" spans="2:27">
       <c r="B34">
         <v>4</v>
       </c>
@@ -1484,8 +1719,18 @@
       <c r="H34" s="36">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:13">
+      <c r="W34" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y34" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:27">
       <c r="B35">
         <v>5</v>
       </c>
@@ -1499,8 +1744,12 @@
       <c r="M35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="2:13">
+      <c r="W35" s="38"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="36"/>
+    </row>
+    <row r="36" spans="2:27">
       <c r="B36">
         <v>6</v>
       </c>
@@ -1511,8 +1760,15 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="36"/>
-    </row>
-    <row r="37" spans="2:13">
+      <c r="W36" s="38"/>
+      <c r="X36" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="36"/>
+    </row>
+    <row r="37" spans="2:27">
       <c r="B37">
         <v>7</v>
       </c>
@@ -1523,8 +1779,15 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="36"/>
-    </row>
-    <row r="38" spans="2:13">
+      <c r="W37" s="38"/>
+      <c r="X37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="36"/>
+    </row>
+    <row r="38" spans="2:27">
       <c r="B38">
         <v>8</v>
       </c>
@@ -1541,8 +1804,18 @@
       <c r="H38" s="36">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="2:13">
+      <c r="X38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27">
       <c r="B39">
         <v>9</v>
       </c>
@@ -1553,8 +1826,14 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="36"/>
-    </row>
-    <row r="40" spans="2:13">
+      <c r="X39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="36"/>
+    </row>
+    <row r="40" spans="2:27">
       <c r="B40">
         <v>10</v>
       </c>
@@ -1568,8 +1847,14 @@
       <c r="M40" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="2:13">
+      <c r="X40" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="36"/>
+    </row>
+    <row r="41" spans="2:27">
       <c r="B41">
         <v>11</v>
       </c>
@@ -1583,8 +1868,12 @@
       <c r="M41" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="2:13">
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
+      <c r="AA41" s="36"/>
+    </row>
+    <row r="42" spans="2:27">
       <c r="B42">
         <v>12</v>
       </c>
@@ -1595,8 +1884,15 @@
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="36"/>
-    </row>
-    <row r="43" spans="2:13">
+      <c r="W42" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="X42" s="7"/>
+      <c r="Y42" s="7"/>
+      <c r="Z42" s="7"/>
+      <c r="AA42" s="36"/>
+    </row>
+    <row r="43" spans="2:27">
       <c r="B43">
         <v>13</v>
       </c>
@@ -1611,8 +1907,18 @@
       <c r="H43" s="36">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="2:13">
+      <c r="W43" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z43" s="7"/>
+      <c r="AA43" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27">
       <c r="B44">
         <v>14</v>
       </c>
@@ -1623,8 +1929,14 @@
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="36"/>
-    </row>
-    <row r="45" spans="2:13">
+      <c r="W44" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="7"/>
+      <c r="Z44" s="7"/>
+      <c r="AA44" s="36"/>
+    </row>
+    <row r="45" spans="2:27">
       <c r="B45">
         <v>15</v>
       </c>
@@ -1635,8 +1947,14 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="36"/>
-    </row>
-    <row r="46" spans="2:13">
+      <c r="W45" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="36"/>
+    </row>
+    <row r="46" spans="2:27">
       <c r="B46">
         <v>16</v>
       </c>
@@ -1647,8 +1965,14 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="36"/>
-    </row>
-    <row r="47" spans="2:13">
+      <c r="W46" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="36"/>
+    </row>
+    <row r="47" spans="2:27">
       <c r="B47">
         <v>17</v>
       </c>
@@ -1665,8 +1989,16 @@
       <c r="H47" s="36">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="2:13">
+      <c r="W47" s="38"/>
+      <c r="Y47" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27">
       <c r="B48">
         <v>18</v>
       </c>
@@ -1677,8 +2009,15 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="36"/>
-    </row>
-    <row r="49" spans="2:8">
+      <c r="W48" s="38"/>
+      <c r="X48" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="36"/>
+    </row>
+    <row r="49" spans="2:27">
       <c r="B49">
         <v>19</v>
       </c>
@@ -1689,8 +2028,15 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="36"/>
-    </row>
-    <row r="50" spans="2:8">
+      <c r="W49" s="38"/>
+      <c r="X49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="36"/>
+    </row>
+    <row r="50" spans="2:27">
       <c r="B50">
         <v>20</v>
       </c>
@@ -1701,8 +2047,15 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="36"/>
-    </row>
-    <row r="51" spans="2:8">
+      <c r="W50" s="38"/>
+      <c r="X50" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="36"/>
+    </row>
+    <row r="51" spans="2:27">
       <c r="B51">
         <v>21</v>
       </c>
@@ -1719,8 +2072,18 @@
       <c r="H51" s="36">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="2:8">
+      <c r="X51" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:27">
       <c r="B52">
         <v>22</v>
       </c>
@@ -1731,8 +2094,14 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="36"/>
-    </row>
-    <row r="53" spans="2:8">
+      <c r="X52" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="36"/>
+    </row>
+    <row r="53" spans="2:27">
       <c r="B53">
         <v>23</v>
       </c>
@@ -1743,8 +2112,11 @@
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="36"/>
-    </row>
-    <row r="54" spans="2:8">
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7"/>
+      <c r="AA53" s="36"/>
+    </row>
+    <row r="54" spans="2:27">
       <c r="B54">
         <v>24</v>
       </c>
@@ -1755,8 +2127,14 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="36"/>
-    </row>
-    <row r="55" spans="2:8">
+      <c r="W54" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="36"/>
+    </row>
+    <row r="55" spans="2:27">
       <c r="B55">
         <v>25</v>
       </c>
@@ -1773,8 +2151,18 @@
       <c r="H55" s="36">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="2:8">
+      <c r="W55" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z55" s="7"/>
+      <c r="AA55" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:27">
       <c r="B56">
         <v>26</v>
       </c>
@@ -1785,8 +2173,14 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="36"/>
-    </row>
-    <row r="57" spans="2:8">
+      <c r="W56" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="36"/>
+    </row>
+    <row r="57" spans="2:27">
       <c r="B57">
         <v>27</v>
       </c>
@@ -1797,8 +2191,14 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="36"/>
-    </row>
-    <row r="58" spans="2:8">
+      <c r="W57" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="36"/>
+    </row>
+    <row r="58" spans="2:27">
       <c r="B58">
         <v>28</v>
       </c>
@@ -1809,8 +2209,14 @@
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="36"/>
-    </row>
-    <row r="59" spans="2:8">
+      <c r="W58" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="36"/>
+    </row>
+    <row r="59" spans="2:27">
       <c r="B59">
         <v>29</v>
       </c>
@@ -1821,8 +2227,11 @@
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="36"/>
-    </row>
-    <row r="60" spans="2:8">
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7"/>
+      <c r="AA59" s="36"/>
+    </row>
+    <row r="60" spans="2:27">
       <c r="B60">
         <v>30</v>
       </c>
@@ -1837,8 +2246,18 @@
       <c r="H60" s="36">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="2:8">
+      <c r="X60" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:27">
       <c r="B61">
         <v>31</v>
       </c>
@@ -1849,8 +2268,14 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="36"/>
-    </row>
-    <row r="62" spans="2:8">
+      <c r="X61" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="36"/>
+    </row>
+    <row r="62" spans="2:27">
       <c r="B62">
         <v>32</v>
       </c>
@@ -1861,8 +2286,14 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="36"/>
-    </row>
-    <row r="63" spans="2:8">
+      <c r="X62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="36"/>
+    </row>
+    <row r="63" spans="2:27">
       <c r="B63">
         <v>33</v>
       </c>
@@ -1873,8 +2304,14 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="36"/>
-    </row>
-    <row r="64" spans="2:8">
+      <c r="X63" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7"/>
+      <c r="AA63" s="36"/>
+    </row>
+    <row r="64" spans="2:27">
       <c r="B64">
         <v>34</v>
       </c>
@@ -1891,8 +2328,18 @@
       <c r="H64" s="36">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="2:8">
+      <c r="X64" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y64" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:27">
       <c r="B65">
         <v>35</v>
       </c>
@@ -1903,8 +2350,11 @@
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="36"/>
-    </row>
-    <row r="66" spans="2:8">
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+      <c r="AA65" s="36"/>
+    </row>
+    <row r="66" spans="2:27">
       <c r="B66">
         <v>36</v>
       </c>
@@ -1915,8 +2365,14 @@
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
       <c r="H66" s="36"/>
-    </row>
-    <row r="67" spans="2:8">
+      <c r="W66" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="7"/>
+      <c r="Z66" s="7"/>
+      <c r="AA66" s="36"/>
+    </row>
+    <row r="67" spans="2:27">
       <c r="B67">
         <v>37</v>
       </c>
@@ -1927,8 +2383,14 @@
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="36"/>
-    </row>
-    <row r="68" spans="2:8">
+      <c r="W67" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7"/>
+      <c r="AA67" s="36"/>
+    </row>
+    <row r="68" spans="2:27">
       <c r="B68">
         <v>38</v>
       </c>
@@ -1945,8 +2407,18 @@
       <c r="H68" s="36">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="2:8">
+      <c r="W68" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y68" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z68" s="7"/>
+      <c r="AA68" s="36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="2:27">
       <c r="B69">
         <v>39</v>
       </c>
@@ -1957,8 +2429,14 @@
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="36"/>
-    </row>
-    <row r="70" spans="2:8">
+      <c r="W69" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7"/>
+      <c r="AA69" s="36"/>
+    </row>
+    <row r="70" spans="2:27">
       <c r="B70">
         <v>40</v>
       </c>
@@ -1969,8 +2447,14 @@
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="36"/>
-    </row>
-    <row r="71" spans="2:8">
+      <c r="W70" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y70" s="7"/>
+      <c r="Z70" s="7"/>
+      <c r="AA70" s="36"/>
+    </row>
+    <row r="71" spans="2:27">
       <c r="B71">
         <v>41</v>
       </c>
@@ -1981,8 +2465,12 @@
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="36"/>
-    </row>
-    <row r="72" spans="2:8">
+      <c r="W71" s="38"/>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="36"/>
+    </row>
+    <row r="72" spans="2:27">
       <c r="B72">
         <v>42</v>
       </c>
@@ -1999,8 +2487,18 @@
       <c r="H72" s="36">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="2:8">
+      <c r="X72" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y72" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:27">
       <c r="B73">
         <v>43</v>
       </c>
@@ -2011,8 +2509,14 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="36"/>
-    </row>
-    <row r="74" spans="2:8">
+      <c r="X73" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="7"/>
+      <c r="AA73" s="36"/>
+    </row>
+    <row r="74" spans="2:27">
       <c r="B74">
         <v>44</v>
       </c>
@@ -2023,8 +2527,14 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="36"/>
-    </row>
-    <row r="75" spans="2:8">
+      <c r="X74" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y74" s="7"/>
+      <c r="Z74" s="7"/>
+      <c r="AA74" s="36"/>
+    </row>
+    <row r="75" spans="2:27">
       <c r="B75">
         <v>45</v>
       </c>
@@ -2035,8 +2545,14 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="36"/>
-    </row>
-    <row r="76" spans="2:8">
+      <c r="X75" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7"/>
+      <c r="AA75" s="36"/>
+    </row>
+    <row r="76" spans="2:27">
       <c r="B76">
         <v>46</v>
       </c>
@@ -2053,8 +2569,18 @@
       <c r="H76" s="36">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="2:8">
+      <c r="X76" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y76" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z76" s="7"/>
+      <c r="AA76" s="36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="2:27">
       <c r="B77">
         <v>47</v>
       </c>
@@ -2065,8 +2591,12 @@
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="36"/>
-    </row>
-    <row r="78" spans="2:8">
+      <c r="X77" s="7"/>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7"/>
+      <c r="AA77" s="36"/>
+    </row>
+    <row r="78" spans="2:27">
       <c r="B78">
         <v>48</v>
       </c>
@@ -2077,8 +2607,15 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="36"/>
-    </row>
-    <row r="79" spans="2:8">
+      <c r="W78" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="X78" s="7"/>
+      <c r="Y78" s="7"/>
+      <c r="Z78" s="7"/>
+      <c r="AA78" s="36"/>
+    </row>
+    <row r="79" spans="2:27">
       <c r="B79">
         <v>49</v>
       </c>
@@ -2089,8 +2626,15 @@
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="36"/>
-    </row>
-    <row r="80" spans="2:8">
+      <c r="W79" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X79" s="7"/>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7"/>
+      <c r="AA79" s="36"/>
+    </row>
+    <row r="80" spans="2:27">
       <c r="B80">
         <v>50</v>
       </c>
@@ -2107,8 +2651,18 @@
       <c r="H80" s="36">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="2:8">
+      <c r="W80" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y80" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z80" s="7"/>
+      <c r="AA80" s="36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="2:27">
       <c r="B81">
         <v>51</v>
       </c>
@@ -2119,8 +2673,14 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
       <c r="H81" s="36"/>
-    </row>
-    <row r="82" spans="2:8">
+      <c r="W81" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="36"/>
+    </row>
+    <row r="82" spans="2:27">
       <c r="B82">
         <v>52</v>
       </c>
@@ -2131,8 +2691,14 @@
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
       <c r="H82" s="36"/>
-    </row>
-    <row r="83" spans="2:8">
+      <c r="W82" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y82" s="7"/>
+      <c r="Z82" s="7"/>
+      <c r="AA82" s="36"/>
+    </row>
+    <row r="83" spans="2:27">
       <c r="B83">
         <v>53</v>
       </c>
@@ -2143,8 +2709,12 @@
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
       <c r="H83" s="36"/>
-    </row>
-    <row r="84" spans="2:8">
+      <c r="W83" s="38"/>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7"/>
+      <c r="AA83" s="36"/>
+    </row>
+    <row r="84" spans="2:27">
       <c r="B84">
         <v>54</v>
       </c>
@@ -2155,8 +2725,15 @@
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="36"/>
-    </row>
-    <row r="85" spans="2:8">
+      <c r="W84" s="38"/>
+      <c r="X84" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y84" s="7"/>
+      <c r="Z84" s="7"/>
+      <c r="AA84" s="36"/>
+    </row>
+    <row r="85" spans="2:27">
       <c r="B85">
         <v>55</v>
       </c>
@@ -2171,8 +2748,19 @@
       <c r="H85" s="36">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="2:8">
+      <c r="W85" s="38"/>
+      <c r="X85" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y85" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z85" s="7"/>
+      <c r="AA85" s="36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="2:27">
       <c r="B86">
         <v>56</v>
       </c>
@@ -2183,8 +2771,14 @@
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="H86" s="36"/>
-    </row>
-    <row r="87" spans="2:8">
+      <c r="X86" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="36"/>
+    </row>
+    <row r="87" spans="2:27">
       <c r="B87">
         <v>57</v>
       </c>
@@ -2195,8 +2789,14 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="36"/>
-    </row>
-    <row r="88" spans="2:8">
+      <c r="X87" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7"/>
+      <c r="AA87" s="36"/>
+    </row>
+    <row r="88" spans="2:27">
       <c r="B88">
         <v>58</v>
       </c>
@@ -2207,8 +2807,14 @@
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="36"/>
-    </row>
-    <row r="89" spans="2:8">
+      <c r="X88" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y88" s="7"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="36"/>
+    </row>
+    <row r="89" spans="2:27">
       <c r="B89">
         <v>59</v>
       </c>
@@ -2225,8 +2831,16 @@
       <c r="H89" s="36">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="2:8">
+      <c r="X89" s="7"/>
+      <c r="Y89" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z89" s="7"/>
+      <c r="AA89" s="36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="2:27">
       <c r="B90">
         <v>60</v>
       </c>
@@ -2237,8 +2851,15 @@
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="H90" s="36"/>
-    </row>
-    <row r="91" spans="2:8">
+      <c r="W90" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="X90" s="7"/>
+      <c r="Y90" s="7"/>
+      <c r="Z90" s="7"/>
+      <c r="AA90" s="36"/>
+    </row>
+    <row r="91" spans="2:27">
       <c r="B91">
         <v>61</v>
       </c>
@@ -2249,8 +2870,15 @@
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="36"/>
-    </row>
-    <row r="92" spans="2:8">
+      <c r="W91" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X91" s="7"/>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7"/>
+      <c r="AA91" s="36"/>
+    </row>
+    <row r="92" spans="2:27">
       <c r="B92">
         <v>62</v>
       </c>
@@ -2261,8 +2889,14 @@
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="36"/>
-    </row>
-    <row r="93" spans="2:8">
+      <c r="W92" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y92" s="7"/>
+      <c r="Z92" s="7"/>
+      <c r="AA92" s="36"/>
+    </row>
+    <row r="93" spans="2:27">
       <c r="B93">
         <v>63</v>
       </c>
@@ -2279,8 +2913,18 @@
       <c r="H93" s="36">
         <v>16</v>
       </c>
-    </row>
-    <row r="94" spans="2:8">
+      <c r="W93" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y93" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z93" s="7"/>
+      <c r="AA93" s="36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="2:27">
       <c r="B94">
         <v>64</v>
       </c>
@@ -2291,8 +2935,14 @@
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="36"/>
-    </row>
-    <row r="95" spans="2:8">
+      <c r="W94" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y94" s="7"/>
+      <c r="Z94" s="7"/>
+      <c r="AA94" s="36"/>
+    </row>
+    <row r="95" spans="2:27">
       <c r="B95">
         <v>65</v>
       </c>
@@ -2303,8 +2953,12 @@
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="36"/>
-    </row>
-    <row r="96" spans="2:8">
+      <c r="W95" s="38"/>
+      <c r="Y95" s="7"/>
+      <c r="Z95" s="7"/>
+      <c r="AA95" s="36"/>
+    </row>
+    <row r="96" spans="2:27">
       <c r="B96">
         <v>66</v>
       </c>
@@ -2315,8 +2969,15 @@
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="36"/>
-    </row>
-    <row r="97" spans="2:10">
+      <c r="W96" s="38"/>
+      <c r="X96" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y96" s="7"/>
+      <c r="Z96" s="7"/>
+      <c r="AA96" s="36"/>
+    </row>
+    <row r="97" spans="2:27">
       <c r="B97">
         <v>67</v>
       </c>
@@ -2327,8 +2988,15 @@
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
       <c r="H97" s="36"/>
-    </row>
-    <row r="98" spans="2:10">
+      <c r="W97" s="38"/>
+      <c r="X97" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7"/>
+      <c r="AA97" s="36"/>
+    </row>
+    <row r="98" spans="2:27">
       <c r="B98">
         <v>68</v>
       </c>
@@ -2343,8 +3011,18 @@
       <c r="H98" s="36">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="2:10">
+      <c r="X98" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y98" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z98" s="7"/>
+      <c r="AA98" s="36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="2:27">
       <c r="B99">
         <v>69</v>
       </c>
@@ -2355,8 +3033,14 @@
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
       <c r="H99" s="36"/>
-    </row>
-    <row r="100" spans="2:10">
+      <c r="X99" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y99" s="7"/>
+      <c r="Z99" s="7"/>
+      <c r="AA99" s="36"/>
+    </row>
+    <row r="100" spans="2:27">
       <c r="B100">
         <v>70</v>
       </c>
@@ -2367,8 +3051,14 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
       <c r="H100" s="36"/>
-    </row>
-    <row r="101" spans="2:10">
+      <c r="X100" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y100" s="7"/>
+      <c r="Z100" s="7"/>
+      <c r="AA100" s="36"/>
+    </row>
+    <row r="101" spans="2:27">
       <c r="B101">
         <v>71</v>
       </c>
@@ -2379,8 +3069,12 @@
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
       <c r="H101" s="36"/>
-    </row>
-    <row r="102" spans="2:10">
+      <c r="X101" s="7"/>
+      <c r="Y101" s="7"/>
+      <c r="Z101" s="7"/>
+      <c r="AA101" s="36"/>
+    </row>
+    <row r="102" spans="2:27">
       <c r="B102">
         <v>72</v>
       </c>
@@ -2397,8 +3091,19 @@
       <c r="H102" s="36">
         <v>18</v>
       </c>
-    </row>
-    <row r="103" spans="2:10">
+      <c r="W102" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="X102" s="7"/>
+      <c r="Y102" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z102" s="7"/>
+      <c r="AA102" s="36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="2:27">
       <c r="B103">
         <v>73</v>
       </c>
@@ -2409,8 +3114,15 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
       <c r="H103" s="36"/>
-    </row>
-    <row r="104" spans="2:10">
+      <c r="W103" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X103" s="7"/>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7"/>
+      <c r="AA103" s="36"/>
+    </row>
+    <row r="104" spans="2:27">
       <c r="B104">
         <v>74</v>
       </c>
@@ -2421,8 +3133,15 @@
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
       <c r="H104" s="36"/>
-    </row>
-    <row r="105" spans="2:10">
+      <c r="W104" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X104" s="7"/>
+      <c r="Y104" s="7"/>
+      <c r="Z104" s="7"/>
+      <c r="AA104" s="36"/>
+    </row>
+    <row r="105" spans="2:27">
       <c r="B105">
         <v>75</v>
       </c>
@@ -2433,8 +3152,14 @@
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
       <c r="H105" s="36"/>
-    </row>
-    <row r="106" spans="2:10">
+      <c r="W105" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y105" s="7"/>
+      <c r="Z105" s="7"/>
+      <c r="AA105" s="36"/>
+    </row>
+    <row r="106" spans="2:27">
       <c r="B106">
         <v>76</v>
       </c>
@@ -2445,8 +3170,14 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="36"/>
-    </row>
-    <row r="107" spans="2:10">
+      <c r="W106" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y106" s="7"/>
+      <c r="Z106" s="7"/>
+      <c r="AA106" s="36"/>
+    </row>
+    <row r="107" spans="2:27">
       <c r="B107">
         <v>77</v>
       </c>
@@ -2455,8 +3186,15 @@
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
       <c r="H107" s="36"/>
-    </row>
-    <row r="108" spans="2:10" ht="15" customHeight="1">
+      <c r="I107" s="47">
+        <v>1</v>
+      </c>
+      <c r="W107" s="38"/>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7"/>
+      <c r="AA107" s="36"/>
+    </row>
+    <row r="108" spans="2:27" ht="15" customHeight="1">
       <c r="B108">
         <v>78</v>
       </c>
@@ -2465,10 +3203,19 @@
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
       <c r="H108" s="42"/>
-      <c r="I108" s="30"/>
+      <c r="I108" s="48">
+        <v>2</v>
+      </c>
       <c r="J108" s="30"/>
-    </row>
-    <row r="109" spans="2:10" ht="15" customHeight="1">
+      <c r="W108" s="38"/>
+      <c r="X108" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y108" s="7"/>
+      <c r="Z108" s="7"/>
+      <c r="AA108" s="42"/>
+    </row>
+    <row r="109" spans="2:27" ht="15" customHeight="1">
       <c r="B109">
         <v>79</v>
       </c>
@@ -2477,10 +3224,19 @@
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
       <c r="H109" s="42"/>
-      <c r="I109" s="30"/>
+      <c r="I109" s="47">
+        <v>3</v>
+      </c>
       <c r="J109" s="30"/>
-    </row>
-    <row r="110" spans="2:10" ht="15" customHeight="1">
+      <c r="W109" s="38"/>
+      <c r="X109" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y109" s="7"/>
+      <c r="Z109" s="7"/>
+      <c r="AA109" s="42"/>
+    </row>
+    <row r="110" spans="2:27" ht="15" customHeight="1">
       <c r="B110">
         <v>80</v>
       </c>
@@ -2489,10 +3245,19 @@
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
       <c r="H110" s="42"/>
-      <c r="I110" s="30"/>
+      <c r="I110" s="48">
+        <v>4</v>
+      </c>
       <c r="J110" s="30"/>
-    </row>
-    <row r="111" spans="2:10" ht="15" customHeight="1">
+      <c r="W110" s="38"/>
+      <c r="X110" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y110" s="7"/>
+      <c r="Z110" s="7"/>
+      <c r="AA110" s="42"/>
+    </row>
+    <row r="111" spans="2:27" ht="15" customHeight="1">
       <c r="B111">
         <v>81</v>
       </c>
@@ -2501,10 +3266,18 @@
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
       <c r="H111" s="42"/>
-      <c r="I111" s="30"/>
+      <c r="I111" s="47">
+        <v>5</v>
+      </c>
       <c r="J111" s="30"/>
-    </row>
-    <row r="112" spans="2:10" ht="15" customHeight="1">
+      <c r="X111" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y111" s="7"/>
+      <c r="Z111" s="7"/>
+      <c r="AA111" s="42"/>
+    </row>
+    <row r="112" spans="2:27" ht="15" customHeight="1">
       <c r="B112">
         <v>82</v>
       </c>
@@ -2513,10 +3286,18 @@
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
       <c r="H112" s="42"/>
-      <c r="I112" s="30"/>
+      <c r="I112" s="48">
+        <v>6</v>
+      </c>
       <c r="J112" s="30"/>
-    </row>
-    <row r="113" spans="2:10" ht="15" customHeight="1">
+      <c r="X112" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y112" s="7"/>
+      <c r="Z112" s="7"/>
+      <c r="AA112" s="42"/>
+    </row>
+    <row r="113" spans="2:27" ht="15" customHeight="1">
       <c r="B113">
         <v>83</v>
       </c>
@@ -2525,10 +3306,16 @@
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
       <c r="H113" s="42"/>
-      <c r="I113" s="30"/>
+      <c r="I113" s="47">
+        <v>7</v>
+      </c>
       <c r="J113" s="30"/>
-    </row>
-    <row r="114" spans="2:10" ht="15" customHeight="1">
+      <c r="X113" s="7"/>
+      <c r="Y113" s="7"/>
+      <c r="Z113" s="7"/>
+      <c r="AA113" s="42"/>
+    </row>
+    <row r="114" spans="2:27" ht="15" customHeight="1">
       <c r="B114">
         <v>84</v>
       </c>
@@ -2537,10 +3324,19 @@
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
       <c r="H114" s="42"/>
-      <c r="I114" s="30"/>
+      <c r="I114" s="48">
+        <v>8</v>
+      </c>
       <c r="J114" s="30"/>
-    </row>
-    <row r="115" spans="2:10" ht="15" customHeight="1">
+      <c r="W114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="X114" s="7"/>
+      <c r="Y114" s="7"/>
+      <c r="Z114" s="7"/>
+      <c r="AA114" s="42"/>
+    </row>
+    <row r="115" spans="2:27" ht="15" customHeight="1">
       <c r="B115">
         <v>85</v>
       </c>
@@ -2549,10 +3345,22 @@
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
       <c r="H115" s="42"/>
-      <c r="I115" s="30"/>
+      <c r="I115" s="47">
+        <v>9</v>
+      </c>
       <c r="J115" s="30"/>
-    </row>
-    <row r="116" spans="2:10" ht="15" customHeight="1">
+      <c r="L115" t="s">
+        <v>29</v>
+      </c>
+      <c r="W115" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="X115" s="7"/>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7"/>
+      <c r="AA115" s="42"/>
+    </row>
+    <row r="116" spans="2:27" ht="15" customHeight="1">
       <c r="B116">
         <v>86</v>
       </c>
@@ -2561,10 +3369,22 @@
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
       <c r="H116" s="42"/>
-      <c r="I116" s="30"/>
+      <c r="I116" s="48">
+        <v>10</v>
+      </c>
       <c r="J116" s="30"/>
-    </row>
-    <row r="117" spans="2:10" ht="15" customHeight="1">
+      <c r="L116" t="str">
+        <f>"+2 Cycle to expand CD Write"</f>
+        <v>+2 Cycle to expand CD Write</v>
+      </c>
+      <c r="W116" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y116" s="7"/>
+      <c r="Z116" s="7"/>
+      <c r="AA116" s="42"/>
+    </row>
+    <row r="117" spans="2:27" ht="15" customHeight="1">
       <c r="B117">
         <v>87</v>
       </c>
@@ -2573,10 +3393,18 @@
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
       <c r="H117" s="42"/>
-      <c r="I117" s="30"/>
+      <c r="I117" s="47">
+        <v>11</v>
+      </c>
       <c r="J117" s="30"/>
-    </row>
-    <row r="118" spans="2:10" ht="15" customHeight="1">
+      <c r="W117" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7"/>
+      <c r="AA117" s="42"/>
+    </row>
+    <row r="118" spans="2:27" ht="15" customHeight="1">
       <c r="B118">
         <v>88</v>
       </c>
@@ -2585,10 +3413,18 @@
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
       <c r="H118" s="42"/>
-      <c r="I118" s="30"/>
+      <c r="I118" s="48">
+        <v>12</v>
+      </c>
       <c r="J118" s="30"/>
-    </row>
-    <row r="119" spans="2:10" ht="15" customHeight="1">
+      <c r="W118" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y118" s="7"/>
+      <c r="Z118" s="7"/>
+      <c r="AA118" s="42"/>
+    </row>
+    <row r="119" spans="2:27" ht="15" customHeight="1">
       <c r="B119">
         <v>89</v>
       </c>
@@ -2597,10 +3433,16 @@
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
       <c r="H119" s="42"/>
-      <c r="I119" s="30"/>
+      <c r="I119" s="47">
+        <v>13</v>
+      </c>
       <c r="J119" s="30"/>
-    </row>
-    <row r="120" spans="2:10" ht="15" customHeight="1">
+      <c r="W119" s="38"/>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7"/>
+      <c r="AA119" s="42"/>
+    </row>
+    <row r="120" spans="2:27" ht="15" customHeight="1">
       <c r="B120">
         <v>90</v>
       </c>
@@ -2609,10 +3451,22 @@
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
       <c r="H120" s="42"/>
-      <c r="I120" s="30"/>
+      <c r="I120" s="48">
+        <v>14</v>
+      </c>
       <c r="J120" s="30"/>
-    </row>
-    <row r="121" spans="2:10" ht="15" customHeight="1">
+      <c r="L120">
+        <v>44</v>
+      </c>
+      <c r="W120" s="38"/>
+      <c r="X120" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="7"/>
+      <c r="Z120" s="7"/>
+      <c r="AA120" s="42"/>
+    </row>
+    <row r="121" spans="2:27" ht="15" customHeight="1">
       <c r="B121">
         <v>91</v>
       </c>
@@ -2621,10 +3475,22 @@
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
       <c r="H121" s="42"/>
-      <c r="I121" s="30"/>
+      <c r="I121" s="47">
+        <v>15</v>
+      </c>
       <c r="J121" s="30"/>
-    </row>
-    <row r="122" spans="2:10" ht="15" customHeight="1">
+      <c r="L121">
+        <v>16</v>
+      </c>
+      <c r="W121" s="38"/>
+      <c r="X121" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7"/>
+      <c r="AA121" s="42"/>
+    </row>
+    <row r="122" spans="2:27" ht="15" customHeight="1">
       <c r="B122">
         <v>92</v>
       </c>
@@ -2633,10 +3499,23 @@
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
       <c r="H122" s="42"/>
-      <c r="I122" s="30"/>
+      <c r="I122" s="48">
+        <v>16</v>
+      </c>
       <c r="J122" s="30"/>
-    </row>
-    <row r="123" spans="2:10" ht="15" customHeight="1">
+      <c r="L122">
+        <f>L120-L121</f>
+        <v>28</v>
+      </c>
+      <c r="W122" s="38"/>
+      <c r="X122" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y122" s="7"/>
+      <c r="Z122" s="7"/>
+      <c r="AA122" s="42"/>
+    </row>
+    <row r="123" spans="2:27" ht="15" customHeight="1">
       <c r="B123">
         <v>93</v>
       </c>
@@ -2645,10 +3524,18 @@
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
       <c r="H123" s="42"/>
-      <c r="I123" s="30"/>
+      <c r="I123" s="47">
+        <v>17</v>
+      </c>
       <c r="J123" s="30"/>
-    </row>
-    <row r="124" spans="2:10" ht="15" customHeight="1">
+      <c r="X123" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7"/>
+      <c r="AA123" s="42"/>
+    </row>
+    <row r="124" spans="2:27" ht="15" customHeight="1">
       <c r="B124">
         <v>94</v>
       </c>
@@ -2657,10 +3544,21 @@
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
       <c r="H124" s="42"/>
-      <c r="I124" s="30"/>
+      <c r="I124" s="48">
+        <v>18</v>
+      </c>
       <c r="J124" s="30"/>
-    </row>
-    <row r="125" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="L124" t="s">
+        <v>30</v>
+      </c>
+      <c r="X124" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y124" s="7"/>
+      <c r="Z124" s="7"/>
+      <c r="AA124" s="42"/>
+    </row>
+    <row r="125" spans="2:27" ht="15.75" customHeight="1" thickBot="1">
       <c r="B125">
         <v>95</v>
       </c>
@@ -2669,10 +3567,20 @@
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="42"/>
-      <c r="I125" s="30"/>
+      <c r="I125" s="47">
+        <v>19</v>
+      </c>
       <c r="J125" s="30"/>
-    </row>
-    <row r="126" spans="2:10" ht="15" customHeight="1">
+      <c r="L125" t="str">
+        <f>"28-24"</f>
+        <v>28-24</v>
+      </c>
+      <c r="X125" s="7"/>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7"/>
+      <c r="AA125" s="42"/>
+    </row>
+    <row r="126" spans="2:27" ht="15" customHeight="1">
       <c r="B126">
         <v>96</v>
       </c>
@@ -2685,10 +3593,21 @@
       <c r="H126" s="36">
         <v>19</v>
       </c>
-      <c r="I126" s="30"/>
+      <c r="I126" s="48"/>
       <c r="J126" s="30"/>
-    </row>
-    <row r="127" spans="2:10" ht="15" customHeight="1">
+      <c r="L126" t="s">
+        <v>31</v>
+      </c>
+      <c r="W126" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y126" s="7"/>
+      <c r="Z126" s="7"/>
+      <c r="AA126" s="36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="2:27" ht="15" customHeight="1">
       <c r="B127">
         <v>97</v>
       </c>
@@ -2699,10 +3618,16 @@
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="42"/>
-      <c r="I127" s="30"/>
+      <c r="I127" s="48"/>
       <c r="J127" s="30"/>
-    </row>
-    <row r="128" spans="2:10" ht="15" customHeight="1">
+      <c r="W127" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7"/>
+      <c r="AA127" s="42"/>
+    </row>
+    <row r="128" spans="2:27" ht="15" customHeight="1">
       <c r="B128">
         <v>98</v>
       </c>
@@ -2713,10 +3638,16 @@
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
       <c r="H128" s="42"/>
-      <c r="I128" s="30"/>
+      <c r="I128" s="48"/>
       <c r="J128" s="30"/>
-    </row>
-    <row r="129" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="W128" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y128" s="7"/>
+      <c r="Z128" s="7"/>
+      <c r="AA128" s="42"/>
+    </row>
+    <row r="129" spans="2:27" ht="15.75" customHeight="1" thickBot="1">
       <c r="B129">
         <v>99</v>
       </c>
@@ -2727,10 +3658,19 @@
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
       <c r="H129" s="42"/>
-      <c r="I129" s="30"/>
+      <c r="I129" s="48"/>
       <c r="J129" s="30"/>
-    </row>
-    <row r="130" spans="2:10" ht="15" customHeight="1">
+      <c r="L129" t="s">
+        <v>32</v>
+      </c>
+      <c r="W129" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y129" s="7"/>
+      <c r="Z129" s="7"/>
+      <c r="AA129" s="42"/>
+    </row>
+    <row r="130" spans="2:27" ht="15" customHeight="1">
       <c r="B130">
         <v>100</v>
       </c>
@@ -2743,10 +3683,19 @@
       <c r="H130" s="36">
         <v>20</v>
       </c>
-      <c r="I130" s="30"/>
+      <c r="I130" s="48"/>
       <c r="J130" s="30"/>
-    </row>
-    <row r="131" spans="2:10" ht="15" customHeight="1">
+      <c r="W130" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="X130" s="7"/>
+      <c r="Y130" s="7"/>
+      <c r="Z130" s="7"/>
+      <c r="AA130" s="36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="2:27" ht="15" customHeight="1">
       <c r="B131">
         <v>101</v>
       </c>
@@ -2757,10 +3706,15 @@
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
       <c r="H131" s="42"/>
-      <c r="I131" s="30"/>
+      <c r="I131" s="48"/>
       <c r="J131" s="30"/>
-    </row>
-    <row r="132" spans="2:10" ht="15" customHeight="1">
+      <c r="W131" s="38"/>
+      <c r="X131" s="7"/>
+      <c r="Y131" s="7"/>
+      <c r="Z131" s="7"/>
+      <c r="AA131" s="42"/>
+    </row>
+    <row r="132" spans="2:27" ht="15" customHeight="1">
       <c r="B132">
         <v>102</v>
       </c>
@@ -2771,10 +3725,17 @@
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
       <c r="H132" s="42"/>
-      <c r="I132" s="30"/>
+      <c r="I132" s="48"/>
       <c r="J132" s="30"/>
-    </row>
-    <row r="133" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="W132" s="41"/>
+      <c r="X132" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y132" s="7"/>
+      <c r="Z132" s="7"/>
+      <c r="AA132" s="42"/>
+    </row>
+    <row r="133" spans="2:27" ht="15.75" customHeight="1" thickBot="1">
       <c r="B133">
         <v>103</v>
       </c>
@@ -2785,10 +3746,17 @@
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
       <c r="H133" s="42"/>
-      <c r="I133" s="30"/>
+      <c r="I133" s="48"/>
       <c r="J133" s="30"/>
-    </row>
-    <row r="134" spans="2:10" ht="15" customHeight="1">
+      <c r="W133" s="41"/>
+      <c r="X133" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7"/>
+      <c r="AA133" s="42"/>
+    </row>
+    <row r="134" spans="2:27" ht="15" customHeight="1">
       <c r="B134">
         <v>104</v>
       </c>
@@ -2797,10 +3765,19 @@
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
       <c r="H134" s="42"/>
-      <c r="I134" s="30"/>
+      <c r="I134" s="48">
+        <v>20</v>
+      </c>
       <c r="J134" s="30"/>
-    </row>
-    <row r="135" spans="2:10" ht="15" customHeight="1">
+      <c r="W134" s="41"/>
+      <c r="X134" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y134" s="7"/>
+      <c r="Z134" s="7"/>
+      <c r="AA134" s="42"/>
+    </row>
+    <row r="135" spans="2:27" ht="15" customHeight="1">
       <c r="B135">
         <v>105</v>
       </c>
@@ -2809,10 +3786,19 @@
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
       <c r="H135" s="42"/>
-      <c r="I135" s="30"/>
+      <c r="I135" s="48">
+        <v>21</v>
+      </c>
       <c r="J135" s="30"/>
-    </row>
-    <row r="136" spans="2:10" ht="15" customHeight="1">
+      <c r="W135" s="41"/>
+      <c r="X135" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y135" s="7"/>
+      <c r="Z135" s="7"/>
+      <c r="AA135" s="42"/>
+    </row>
+    <row r="136" spans="2:27" ht="15" customHeight="1">
       <c r="B136">
         <v>106</v>
       </c>
@@ -2821,10 +3807,19 @@
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
       <c r="H136" s="42"/>
-      <c r="I136" s="30"/>
+      <c r="I136" s="48">
+        <v>22</v>
+      </c>
       <c r="J136" s="30"/>
-    </row>
-    <row r="137" spans="2:10" ht="15" customHeight="1">
+      <c r="W136" s="41"/>
+      <c r="X136" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y136" s="7"/>
+      <c r="Z136" s="7"/>
+      <c r="AA136" s="42"/>
+    </row>
+    <row r="137" spans="2:27" ht="15" customHeight="1" thickBot="1">
       <c r="B137">
         <v>107</v>
       </c>
@@ -2833,10 +3828,16 @@
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="42"/>
-      <c r="I137" s="30"/>
+      <c r="I137" s="48">
+        <v>23</v>
+      </c>
       <c r="J137" s="30"/>
-    </row>
-    <row r="138" spans="2:10" ht="15" customHeight="1">
+      <c r="W137" s="41"/>
+      <c r="Y137" s="7"/>
+      <c r="Z137" s="7"/>
+      <c r="AA137" s="42"/>
+    </row>
+    <row r="138" spans="2:27" ht="15" customHeight="1">
       <c r="B138">
         <v>108</v>
       </c>
@@ -2845,10 +3846,19 @@
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
       <c r="H138" s="42"/>
-      <c r="I138" s="30"/>
+      <c r="I138" s="48">
+        <v>24</v>
+      </c>
       <c r="J138" s="30"/>
-    </row>
-    <row r="139" spans="2:10" ht="15" customHeight="1">
+      <c r="W138" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="X138" s="31"/>
+      <c r="Y138" s="7"/>
+      <c r="Z138" s="7"/>
+      <c r="AA138" s="42"/>
+    </row>
+    <row r="139" spans="2:27" ht="15" customHeight="1">
       <c r="B139">
         <v>109</v>
       </c>
@@ -2857,10 +3867,19 @@
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
       <c r="H139" s="42"/>
-      <c r="I139" s="30"/>
+      <c r="I139" s="48">
+        <v>25</v>
+      </c>
       <c r="J139" s="30"/>
-    </row>
-    <row r="140" spans="2:10" ht="15" customHeight="1">
+      <c r="W139" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X139" s="31"/>
+      <c r="Y139" s="7"/>
+      <c r="Z139" s="7"/>
+      <c r="AA139" s="42"/>
+    </row>
+    <row r="140" spans="2:27" ht="15" customHeight="1">
       <c r="B140">
         <v>110</v>
       </c>
@@ -2869,10 +3888,19 @@
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
       <c r="H140" s="42"/>
-      <c r="I140" s="30"/>
+      <c r="I140" s="48">
+        <v>26</v>
+      </c>
       <c r="J140" s="30"/>
-    </row>
-    <row r="141" spans="2:10" ht="15" customHeight="1">
+      <c r="W140" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X140" s="31"/>
+      <c r="Y140" s="7"/>
+      <c r="Z140" s="7"/>
+      <c r="AA140" s="42"/>
+    </row>
+    <row r="141" spans="2:27" ht="15" customHeight="1" thickBot="1">
       <c r="B141">
         <v>111</v>
       </c>
@@ -2881,10 +3909,19 @@
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="42"/>
-      <c r="I141" s="30"/>
+      <c r="I141" s="48">
+        <v>27</v>
+      </c>
       <c r="J141" s="30"/>
-    </row>
-    <row r="142" spans="2:10" ht="15" customHeight="1">
+      <c r="W141" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="X141" s="31"/>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7"/>
+      <c r="AA141" s="42"/>
+    </row>
+    <row r="142" spans="2:27" ht="15" customHeight="1">
       <c r="B142">
         <v>112</v>
       </c>
@@ -2893,10 +3930,17 @@
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
       <c r="H142" s="42"/>
-      <c r="I142" s="30"/>
+      <c r="I142" s="48">
+        <v>28</v>
+      </c>
       <c r="J142" s="30"/>
-    </row>
-    <row r="143" spans="2:10" ht="15" customHeight="1">
+      <c r="W142" s="41"/>
+      <c r="X142" s="31"/>
+      <c r="Y142" s="7"/>
+      <c r="Z142" s="7"/>
+      <c r="AA142" s="42"/>
+    </row>
+    <row r="143" spans="2:27" ht="15" customHeight="1" thickBot="1">
       <c r="B143">
         <v>113</v>
       </c>
@@ -2905,10 +3949,17 @@
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="42"/>
-      <c r="I143" s="30"/>
+      <c r="I143" s="48">
+        <v>29</v>
+      </c>
       <c r="J143" s="30"/>
-    </row>
-    <row r="144" spans="2:10" ht="15" customHeight="1">
+      <c r="W143" s="41"/>
+      <c r="X143" s="31"/>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7"/>
+      <c r="AA143" s="42"/>
+    </row>
+    <row r="144" spans="2:27" ht="15" customHeight="1">
       <c r="B144">
         <v>114</v>
       </c>
@@ -2917,10 +3968,19 @@
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
       <c r="H144" s="42"/>
-      <c r="I144" s="30"/>
+      <c r="I144" s="48">
+        <v>30</v>
+      </c>
       <c r="J144" s="30"/>
-    </row>
-    <row r="145" spans="2:10" ht="15" customHeight="1">
+      <c r="W144" s="41"/>
+      <c r="X144" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y144" s="7"/>
+      <c r="Z144" s="7"/>
+      <c r="AA144" s="42"/>
+    </row>
+    <row r="145" spans="2:27" ht="15" customHeight="1">
       <c r="B145">
         <v>115</v>
       </c>
@@ -2929,10 +3989,19 @@
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
       <c r="H145" s="42"/>
-      <c r="I145" s="30"/>
+      <c r="I145" s="48">
+        <v>31</v>
+      </c>
       <c r="J145" s="30"/>
-    </row>
-    <row r="146" spans="2:10" ht="15" customHeight="1">
+      <c r="W145" s="41"/>
+      <c r="X145" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y145" s="7"/>
+      <c r="Z145" s="7"/>
+      <c r="AA145" s="42"/>
+    </row>
+    <row r="146" spans="2:27" ht="15" customHeight="1">
       <c r="B146">
         <v>116</v>
       </c>
@@ -2941,10 +4010,19 @@
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
       <c r="H146" s="42"/>
-      <c r="I146" s="30"/>
+      <c r="I146" s="48">
+        <v>32</v>
+      </c>
       <c r="J146" s="30"/>
-    </row>
-    <row r="147" spans="2:10" ht="15" customHeight="1">
+      <c r="W146" s="41"/>
+      <c r="X146" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y146" s="7"/>
+      <c r="Z146" s="7"/>
+      <c r="AA146" s="42"/>
+    </row>
+    <row r="147" spans="2:27" ht="15" customHeight="1" thickBot="1">
       <c r="B147">
         <v>117</v>
       </c>
@@ -2953,10 +4031,19 @@
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
       <c r="H147" s="42"/>
-      <c r="I147" s="30"/>
+      <c r="I147" s="48">
+        <v>33</v>
+      </c>
       <c r="J147" s="30"/>
-    </row>
-    <row r="148" spans="2:10" ht="15" customHeight="1">
+      <c r="W147" s="41"/>
+      <c r="X147" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y147" s="7"/>
+      <c r="Z147" s="7"/>
+      <c r="AA147" s="42"/>
+    </row>
+    <row r="148" spans="2:27" ht="15" customHeight="1">
       <c r="B148">
         <v>118</v>
       </c>
@@ -2965,10 +4052,17 @@
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
       <c r="H148" s="42"/>
-      <c r="I148" s="30"/>
+      <c r="I148" s="48">
+        <v>34</v>
+      </c>
       <c r="J148" s="30"/>
-    </row>
-    <row r="149" spans="2:10" ht="15" customHeight="1">
+      <c r="W148" s="41"/>
+      <c r="X148" s="31"/>
+      <c r="Y148" s="7"/>
+      <c r="Z148" s="7"/>
+      <c r="AA148" s="42"/>
+    </row>
+    <row r="149" spans="2:27" ht="15" customHeight="1">
       <c r="B149">
         <v>119</v>
       </c>
@@ -2977,10 +4071,17 @@
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
       <c r="H149" s="42"/>
-      <c r="I149" s="30"/>
+      <c r="I149" s="48">
+        <v>35</v>
+      </c>
       <c r="J149" s="30"/>
-    </row>
-    <row r="150" spans="2:10" ht="15" customHeight="1">
+      <c r="W149" s="41"/>
+      <c r="X149" s="31"/>
+      <c r="Y149" s="7"/>
+      <c r="Z149" s="7"/>
+      <c r="AA149" s="42"/>
+    </row>
+    <row r="150" spans="2:27" ht="15" customHeight="1">
       <c r="B150">
         <v>120</v>
       </c>
@@ -2989,10 +4090,17 @@
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
       <c r="H150" s="42"/>
-      <c r="I150" s="30"/>
+      <c r="I150" s="48">
+        <v>36</v>
+      </c>
       <c r="J150" s="30"/>
-    </row>
-    <row r="151" spans="2:10" ht="15" customHeight="1">
+      <c r="W150" s="49"/>
+      <c r="X150" s="50"/>
+      <c r="Y150" s="7"/>
+      <c r="Z150" s="7"/>
+      <c r="AA150" s="42"/>
+    </row>
+    <row r="151" spans="2:27" ht="15" customHeight="1">
       <c r="B151">
         <v>121</v>
       </c>
@@ -3001,10 +4109,17 @@
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
       <c r="H151" s="42"/>
-      <c r="I151" s="30"/>
+      <c r="I151" s="48">
+        <v>37</v>
+      </c>
       <c r="J151" s="30"/>
-    </row>
-    <row r="152" spans="2:10" ht="15" customHeight="1">
+      <c r="W151" s="49"/>
+      <c r="X151" s="50"/>
+      <c r="Y151" s="7"/>
+      <c r="Z151" s="7"/>
+      <c r="AA151" s="42"/>
+    </row>
+    <row r="152" spans="2:27" ht="15" customHeight="1">
       <c r="B152">
         <v>122</v>
       </c>
@@ -3013,10 +4128,17 @@
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
       <c r="H152" s="42"/>
-      <c r="I152" s="30"/>
+      <c r="I152" s="48">
+        <v>38</v>
+      </c>
       <c r="J152" s="30"/>
-    </row>
-    <row r="153" spans="2:10" ht="15" customHeight="1">
+      <c r="W152" s="49"/>
+      <c r="X152" s="50"/>
+      <c r="Y152" s="7"/>
+      <c r="Z152" s="7"/>
+      <c r="AA152" s="42"/>
+    </row>
+    <row r="153" spans="2:27" ht="15" customHeight="1">
       <c r="B153">
         <v>123</v>
       </c>
@@ -3025,10 +4147,17 @@
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
       <c r="H153" s="42"/>
-      <c r="I153" s="30"/>
+      <c r="I153" s="48">
+        <v>39</v>
+      </c>
       <c r="J153" s="30"/>
-    </row>
-    <row r="154" spans="2:10" ht="15" customHeight="1">
+      <c r="W153" s="49"/>
+      <c r="X153" s="50"/>
+      <c r="Y153" s="7"/>
+      <c r="Z153" s="7"/>
+      <c r="AA153" s="42"/>
+    </row>
+    <row r="154" spans="2:27" ht="15" customHeight="1">
       <c r="B154">
         <v>124</v>
       </c>
@@ -3037,10 +4166,17 @@
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
       <c r="H154" s="42"/>
-      <c r="I154" s="30"/>
+      <c r="I154" s="48">
+        <v>40</v>
+      </c>
       <c r="J154" s="30"/>
-    </row>
-    <row r="155" spans="2:10" ht="15" customHeight="1">
+      <c r="W154" s="49"/>
+      <c r="X154" s="50"/>
+      <c r="Y154" s="7"/>
+      <c r="Z154" s="7"/>
+      <c r="AA154" s="42"/>
+    </row>
+    <row r="155" spans="2:27" ht="15" customHeight="1">
       <c r="B155">
         <v>125</v>
       </c>
@@ -3049,10 +4185,17 @@
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
       <c r="H155" s="42"/>
-      <c r="I155" s="30"/>
+      <c r="I155" s="48">
+        <v>41</v>
+      </c>
       <c r="J155" s="30"/>
-    </row>
-    <row r="156" spans="2:10" ht="15" customHeight="1">
+      <c r="W155" s="49"/>
+      <c r="X155" s="50"/>
+      <c r="Y155" s="7"/>
+      <c r="Z155" s="7"/>
+      <c r="AA155" s="42"/>
+    </row>
+    <row r="156" spans="2:27" ht="15" customHeight="1">
       <c r="B156">
         <v>126</v>
       </c>
@@ -3061,10 +4204,17 @@
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
       <c r="H156" s="42"/>
-      <c r="I156" s="30"/>
+      <c r="I156" s="48">
+        <v>42</v>
+      </c>
       <c r="J156" s="30"/>
-    </row>
-    <row r="157" spans="2:10" ht="15" customHeight="1">
+      <c r="W156" s="49"/>
+      <c r="X156" s="50"/>
+      <c r="Y156" s="7"/>
+      <c r="Z156" s="7"/>
+      <c r="AA156" s="42"/>
+    </row>
+    <row r="157" spans="2:27" ht="15" customHeight="1">
       <c r="B157">
         <v>127</v>
       </c>
@@ -3073,10 +4223,17 @@
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
       <c r="H157" s="42"/>
-      <c r="I157" s="30"/>
+      <c r="I157" s="48">
+        <v>43</v>
+      </c>
       <c r="J157" s="30"/>
-    </row>
-    <row r="158" spans="2:10" ht="15" customHeight="1" thickBot="1">
+      <c r="W157" s="49"/>
+      <c r="X157" s="50"/>
+      <c r="Y157" s="7"/>
+      <c r="Z157" s="7"/>
+      <c r="AA157" s="42"/>
+    </row>
+    <row r="158" spans="2:27" ht="15" customHeight="1" thickBot="1">
       <c r="B158">
         <v>128</v>
       </c>
@@ -3085,12 +4242,19 @@
       <c r="F158" s="45"/>
       <c r="G158" s="45"/>
       <c r="H158" s="46"/>
-      <c r="I158" s="30"/>
+      <c r="I158" s="48">
+        <v>44</v>
+      </c>
       <c r="J158" s="30"/>
+      <c r="W158" s="51"/>
+      <c r="X158" s="52"/>
+      <c r="Y158" s="45"/>
+      <c r="Z158" s="45"/>
+      <c r="AA158" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="42" fitToWidth="2" fitToHeight="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" fitToWidth="2" fitToHeight="2" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
- Avocado's SPU reference stand alone. - Updated state machine document. - Non standard input clock support. (Ex. 40 Mhz but output audio at 33.8 Mhz using 40 Mhz clock)
</commit_message>
<xml_diff>
--- a/hdlSPU/doc/StateMachineTiming.xlsx
+++ b/hdlSPU/doc/StateMachineTiming.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="36">
   <si>
     <t>READ ADPCM</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Reduce from 128 to 104 cycles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;== FIFO </t>
+  </si>
+  <si>
+    <t>XFER READ/WRITE</t>
+  </si>
+  <si>
+    <t>MEMORIZE FOR CHANNEL WRITE BACK</t>
   </si>
 </sst>
 </file>
@@ -837,10 +846,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE158"/>
+  <dimension ref="A1:AG158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -851,6 +860,10 @@
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="13" max="17" width="14" customWidth="1"/>
     <col min="23" max="27" width="17.5703125" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" customWidth="1"/>
+    <col min="30" max="30" width="14" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" customWidth="1"/>
+    <col min="33" max="33" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" thickBot="1"/>
@@ -906,6 +919,9 @@
       <c r="AA2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="AC2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:31" ht="15.75" thickBot="1">
       <c r="B3">
@@ -931,6 +947,12 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="25" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:31">
       <c r="B4">
@@ -965,6 +987,12 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="8"/>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:31">
       <c r="B5">
@@ -993,6 +1021,12 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="8"/>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1">
       <c r="B6">
@@ -1021,6 +1055,12 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="8"/>
+      <c r="AB6">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1">
       <c r="B7">
@@ -1046,6 +1086,12 @@
         <v>2</v>
       </c>
       <c r="AA7" s="8"/>
+      <c r="AB7">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1">
       <c r="B8">
@@ -1070,6 +1116,12 @@
       <c r="Q8" s="8"/>
       <c r="W8" s="6"/>
       <c r="AA8" s="8"/>
+      <c r="AB8">
+        <v>5</v>
+      </c>
+      <c r="AC8" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1">
       <c r="B9">
@@ -1092,8 +1144,14 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="8"/>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="AB9">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" thickBot="1">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1123,6 +1181,12 @@
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
+      <c r="AB10">
+        <v>7</v>
+      </c>
+      <c r="AC10" s="27" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:31">
       <c r="B11">
@@ -1151,6 +1215,15 @@
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="8"/>
+      <c r="AB11">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="25" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1">
       <c r="B12">
@@ -1179,6 +1252,12 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="8"/>
+      <c r="AB12">
+        <v>9</v>
+      </c>
+      <c r="AD12" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1">
       <c r="B13">
@@ -1207,6 +1286,12 @@
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="8"/>
+      <c r="AB13">
+        <v>10</v>
+      </c>
+      <c r="AD13" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1">
       <c r="B14">
@@ -1234,6 +1319,12 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="8"/>
+      <c r="AB14">
+        <v>11</v>
+      </c>
+      <c r="AD14" s="26" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1">
       <c r="B15">
@@ -1261,7 +1352,12 @@
       <c r="Y15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AD15" s="7"/>
+      <c r="AB15">
+        <v>12</v>
+      </c>
+      <c r="AD15" s="26" t="s">
+        <v>1</v>
+      </c>
       <c r="AE15" s="7"/>
     </row>
     <row r="16" spans="1:31">
@@ -1295,10 +1391,15 @@
       <c r="Y16" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AD16" s="7"/>
+      <c r="AB16">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="26" t="s">
+        <v>1</v>
+      </c>
       <c r="AE16" s="7"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:33">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1333,9 +1434,15 @@
       <c r="AA17" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="AB17">
+        <v>14</v>
+      </c>
+      <c r="AD17" s="26" t="s">
+        <v>1</v>
+      </c>
       <c r="AE17" s="7"/>
     </row>
-    <row r="18" spans="1:31" ht="15.75" thickBot="1">
+    <row r="18" spans="1:33" ht="15.75" thickBot="1">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1367,9 +1474,15 @@
       <c r="AA18" s="15" t="s">
         <v>7</v>
       </c>
+      <c r="AB18">
+        <v>15</v>
+      </c>
+      <c r="AD18" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="AE18" s="7"/>
     </row>
-    <row r="19" spans="1:31" ht="15.75" thickBot="1">
+    <row r="19" spans="1:33" ht="15.75" thickBot="1">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1401,9 +1514,17 @@
       <c r="AA19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="AE19" s="7"/>
-    </row>
-    <row r="20" spans="1:31">
+      <c r="AB19">
+        <v>16</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1431,9 +1552,17 @@
       <c r="AA20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AE20" s="7"/>
-    </row>
-    <row r="21" spans="1:31" ht="15.75" thickBot="1">
+      <c r="AB20">
+        <v>17</v>
+      </c>
+      <c r="AE20" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" ht="15.75" thickBot="1">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1461,9 +1590,17 @@
       <c r="AA21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="AE21" s="7"/>
-    </row>
-    <row r="22" spans="1:31" ht="15.75" thickBot="1">
+      <c r="AB21">
+        <v>18</v>
+      </c>
+      <c r="AE21" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="15.75" thickBot="1">
       <c r="B22">
         <v>19</v>
       </c>
@@ -1488,9 +1625,18 @@
         <v>13</v>
       </c>
       <c r="AA22" s="8"/>
+      <c r="AB22">
+        <v>19</v>
+      </c>
       <c r="AD22" s="7"/>
-    </row>
-    <row r="23" spans="1:31">
+      <c r="AE22" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
       <c r="B23">
         <v>20</v>
       </c>
@@ -1519,9 +1665,18 @@
         <v>1</v>
       </c>
       <c r="AA23" s="8"/>
+      <c r="AB23">
+        <v>20</v>
+      </c>
       <c r="AD23" s="7"/>
-    </row>
-    <row r="24" spans="1:31">
+      <c r="AE23" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" ht="15.75" thickBot="1">
       <c r="B24">
         <v>21</v>
       </c>
@@ -1547,9 +1702,18 @@
         <v>1</v>
       </c>
       <c r="AA24" s="8"/>
+      <c r="AB24">
+        <v>21</v>
+      </c>
       <c r="AD24" s="7"/>
-    </row>
-    <row r="25" spans="1:31" ht="15.75" thickBot="1">
+      <c r="AE24" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" ht="15.75" thickBot="1">
       <c r="B25">
         <v>22</v>
       </c>
@@ -1572,9 +1736,18 @@
         <v>1</v>
       </c>
       <c r="AA25" s="8"/>
+      <c r="AB25">
+        <v>22</v>
+      </c>
       <c r="AD25" s="7"/>
-    </row>
-    <row r="26" spans="1:31" ht="15.75" thickBot="1">
+      <c r="AE25" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" ht="15.75" thickBot="1">
       <c r="B26">
         <v>23</v>
       </c>
@@ -1592,13 +1765,27 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="1"/>
       <c r="AA26" s="22"/>
-    </row>
-    <row r="28" spans="1:31">
+      <c r="AB26">
+        <v>23</v>
+      </c>
+      <c r="AE26" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
+      <c r="AE27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
       <c r="N28" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="15.75" thickBot="1">
+    <row r="29" spans="1:33" ht="15.75" thickBot="1">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1606,7 +1793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:33">
       <c r="B30">
         <v>0</v>
       </c>
@@ -1636,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:33">
       <c r="B31">
         <v>1</v>
       </c>
@@ -1658,7 +1845,7 @@
       <c r="Z31" s="7"/>
       <c r="AA31" s="36"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:33">
       <c r="B32">
         <v>2</v>
       </c>

</xml_diff>